<commit_message>
Adicionando laço de repetição à tela de cadastro para gerar senhas aleatórias
</commit_message>
<xml_diff>
--- a/Planilha_de_Risco/Planilha_de_Riscos.xlsx
+++ b/Planilha_de_Risco/Planilha_de_Riscos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Projeto_PI\sprint2\Planilha_de_Risco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95B2E4C9-F43C-498C-9C46-420FB02ADF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF30A39-F56D-4710-8E15-90EE79E7E9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DD058C87-4DC8-42DE-967C-2167F8755234}"/>
   </bookViews>
@@ -215,18 +215,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -243,52 +240,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFCB0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -457,6 +408,52 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCB0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -476,18 +473,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{060B6AA6-7F0F-4596-B972-46262FBF38DA}" name="Tabela1" displayName="Tabela1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="10" headerRowBorderDxfId="1" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{060B6AA6-7F0F-4596-B972-46262FBF38DA}" name="Tabela1" displayName="Tabela1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
   <autoFilter ref="A1:G9" xr:uid="{060B6AA6-7F0F-4596-B972-46262FBF38DA}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0ED528E2-79D1-44C6-9FBC-FD59A7B89485}" name="Id" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{F8FD5D8B-E637-4A80-A5D9-879E25D25017}" name="Descrição do Risco" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{1D376EBA-FE0D-40D8-9233-7C98C27D34DF}" name="Probabilidade (P)" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{043BA03D-D3BA-44EE-80E8-4413875DD727}" name="Impacto (I)" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{2AC3B614-57F6-444B-A476-F1245DF81C04}" name="Fator de Risco (P x I)" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{0ED528E2-79D1-44C6-9FBC-FD59A7B89485}" name="Id" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{F8FD5D8B-E637-4A80-A5D9-879E25D25017}" name="Descrição do Risco" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{1D376EBA-FE0D-40D8-9233-7C98C27D34DF}" name="Probabilidade (P)" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{043BA03D-D3BA-44EE-80E8-4413875DD727}" name="Impacto (I)" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{2AC3B614-57F6-444B-A476-F1245DF81C04}" name="Fator de Risco (P x I)" dataDxfId="2">
       <calculatedColumnFormula>C2*D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1E4B3A08-286A-47DA-910D-AF20C9EA6C77}" name="Ação" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{643FE018-2FDA-4074-BBEB-2A3348DDE409}" name="Como?" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{1E4B3A08-286A-47DA-910D-AF20C9EA6C77}" name="Ação" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{643FE018-2FDA-4074-BBEB-2A3348DDE409}" name="Como?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -813,7 +810,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -829,217 +826,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
         <f>C2*D2</f>
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="62" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <f t="shared" ref="E3:E9" si="0">C3*D3</f>
         <v>2</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="62" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="62" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="2">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="2">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="62" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>2</v>
       </c>
-      <c r="D9" s="2">
-        <v>3</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>